<commit_message>
Implemented Webdriver Explicit wait, Added Data Provider and updated pom.xml
</commit_message>
<xml_diff>
--- a/TestData/Register.xlsx
+++ b/TestData/Register.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B871CCA6-FBE7-49FC-BFDA-972139A1FDF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4257EC4B-993B-4472-8495-2CA9B22BB6D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>Auto</t>
   </si>
   <si>
@@ -44,6 +35,15 @@
   </si>
   <si>
     <t>Auto.Reg1rew@yopmail.com</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -119,11 +119,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,38 +453,38 @@
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7ED63F57-644F-4E78-9587-08CB51DEF5FB}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{4D7CF1C6-DA0B-403C-A00D-520D86F64D74}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4D7CF1C6-DA0B-403C-A00D-520D86F64D74}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{7ED63F57-644F-4E78-9587-08CB51DEF5FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>